<commit_message>
historias de usuario ok
</commit_message>
<xml_diff>
--- a/Fase 2/ProductoBacklog.xlsx
+++ b/Fase 2/ProductoBacklog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikoo\Desktop\LicitaLabMobile\Fase 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E13B78-D88E-4244-B63F-5F93A6556A8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BEB6041-8DC2-4806-AAC9-ADE3C46E407A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2160" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Historias de Usuario" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="102">
   <si>
     <t>Columna</t>
   </si>
@@ -296,28 +296,49 @@
     <t>Nicolas/Matias</t>
   </si>
   <si>
-    <t>Cotizaciones y detalles</t>
-  </si>
-  <si>
     <t>Agregar filtro por estado de oportunidad en seguimiento</t>
   </si>
   <si>
-    <t>Configuracion notificaciones</t>
-  </si>
-  <si>
     <t>Integracion notificaciones</t>
   </si>
   <si>
     <t>Ordenes de compras</t>
   </si>
   <si>
-    <t>Sin asignar</t>
-  </si>
-  <si>
     <t>Como usuario, debo recibir mi seguimiento asociado a la aplicacion de LicitaLab web.</t>
   </si>
   <si>
     <t>Como usuario, quiero ver los items que contiene una licitacion</t>
+  </si>
+  <si>
+    <t>pdf ordenes de compras</t>
+  </si>
+  <si>
+    <t>Buscar por id o nombre orden de compras</t>
+  </si>
+  <si>
+    <t>Como usuario,quiero poder filtrar por los diferentes estados que tienen las oportunidades</t>
+  </si>
+  <si>
+    <t>Como usuario, quiero recibir unas alertas que me permitan estar atento a las diferentes oportunidades que tengo en seguimiento</t>
+  </si>
+  <si>
+    <t>Como usuario, quiero poder visualizar los diferentes pdf que contiene la orden de compra.</t>
+  </si>
+  <si>
+    <t>Como usuario, quiero poder filtrar por la id o nombre de las ordenes de compras</t>
+  </si>
+  <si>
+    <t>Competado</t>
+  </si>
+  <si>
+    <t>Filtrar ordenes de compras por estado</t>
+  </si>
+  <si>
+    <t>Como usuario, quiero tener a mano las diferentes órdenes de compra que recibo día a día.</t>
+  </si>
+  <si>
+    <t>Como usario, quiero poder filtrar por los diferentes estados que tienen las ordenes de compras</t>
   </si>
 </sst>
 </file>
@@ -430,7 +451,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -464,6 +485,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -772,7 +795,7 @@
   <dimension ref="B1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23:C25"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1063,7 +1086,7 @@
         <v>30</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D14" s="11" t="s">
         <v>57</v>
@@ -1089,7 +1112,7 @@
         <v>31</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>65</v>
@@ -1251,7 +1274,7 @@
         <v>56</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="F21" s="9">
         <v>3</v>
@@ -1296,118 +1319,154 @@
       <c r="B23" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="2" t="s">
+      <c r="C23" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>87</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F23" s="9"/>
-      <c r="G23" s="7"/>
+        <v>66</v>
+      </c>
+      <c r="F23" s="9">
+        <v>3</v>
+      </c>
+      <c r="G23" s="7">
+        <v>3</v>
+      </c>
       <c r="H23" s="7">
         <v>19</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="5"/>
+      <c r="C24" s="10" t="s">
+        <v>95</v>
+      </c>
       <c r="D24" s="5" t="s">
         <v>88</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F24" s="9"/>
-      <c r="G24" s="7"/>
+        <v>66</v>
+      </c>
+      <c r="F24" s="9">
+        <v>8</v>
+      </c>
+      <c r="G24" s="7">
+        <v>3</v>
+      </c>
       <c r="H24" s="7">
         <v>20</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="5"/>
+      <c r="C25" s="18" t="s">
+        <v>100</v>
+      </c>
       <c r="D25" s="5" t="s">
         <v>89</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F25" s="9"/>
-      <c r="G25" s="7"/>
+        <v>66</v>
+      </c>
+      <c r="F25" s="9">
+        <v>3</v>
+      </c>
+      <c r="G25" s="7">
+        <v>3</v>
+      </c>
       <c r="H25" s="7">
         <v>21</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="5"/>
+      <c r="C26" s="10" t="s">
+        <v>96</v>
+      </c>
       <c r="D26" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F26" s="9"/>
-      <c r="G26" s="7"/>
+        <v>66</v>
+      </c>
+      <c r="F26" s="9">
+        <v>4</v>
+      </c>
+      <c r="G26" s="7">
+        <v>4</v>
+      </c>
       <c r="H26" s="7">
         <v>22</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5" t="s">
-        <v>91</v>
+      <c r="C27" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F27" s="9"/>
-      <c r="G27" s="7"/>
+        <v>98</v>
+      </c>
+      <c r="F27" s="9">
+        <v>3</v>
+      </c>
+      <c r="G27" s="7">
+        <v>4</v>
+      </c>
       <c r="H27" s="7">
         <v>23</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
+      <c r="C28" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>99</v>
+      </c>
       <c r="E28" s="5" t="s">
         <v>42</v>
       </c>
       <c r="F28" s="9"/>
-      <c r="G28" s="7"/>
+      <c r="G28" s="7">
+        <v>5</v>
+      </c>
       <c r="H28" s="7">
         <v>24</v>
       </c>
-      <c r="I28" s="7">
-        <v>24</v>
+      <c r="I28" s="7" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
@@ -1421,12 +1480,8 @@
       </c>
       <c r="F29" s="9"/>
       <c r="G29" s="7"/>
-      <c r="H29" s="7">
-        <v>25</v>
-      </c>
-      <c r="I29" s="7">
-        <v>25</v>
-      </c>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34" s="15"/>

</xml_diff>